<commit_message>
[GENERAL] Adding several files and including files for testing the waterflow sensor
</commit_message>
<xml_diff>
--- a/Waterflow Reading/alternate_flow_sensor/flow_calibration.xlsx
+++ b/Waterflow Reading/alternate_flow_sensor/flow_calibration.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28209"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sdwpearson/Documents/UBC/UBC Year 4/ELEC 491/capstone66/Waterflow Reading/alternate_flow_sensor/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14320" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="60">
   <si>
     <t>Water volume (ml)</t>
   </si>
@@ -31,6 +39,174 @@
   </si>
   <si>
     <t>`</t>
+  </si>
+  <si>
+    <t>&lt;- Legacy Test</t>
+  </si>
+  <si>
+    <t>Super low flow</t>
+  </si>
+  <si>
+    <t>pulse/ml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 23716 WaterFlow: 0.00 ml Flow rate: 0.84 L/min: Pulse count: 3 Pulse Frequency: 3.14 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 24256 WaterFlow: 0.00 ml Flow rate: 1.44 L/min: Pulse count: 6 Pulse Frequency: 5.41 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 24796 WaterFlow: 0.00 ml Flow rate: 1.73 L/min: Pulse count: 9 Pulse Frequency: 6.49 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 25335 WaterFlow: 0.00 ml Flow rate: 2.01 L/min: Pulse count: 11 Pulse Frequency: 3.53 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 25876 WaterFlow: 0.00 ml Flow rate: 5.03 L/min: Pulse count: 18 Pulse Frequency: 18.87 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 26418 WaterFlow: 0.00 ml Flow rate: 7.02 L/min: Pulse count: 31 Pulse Frequency: 27.78 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 26959 WaterFlow: 0.00 ml Flow rate: 7.21 L/min: Pulse count: 46 Pulse Frequency: 27.03 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 27501 WaterFlow: 0.00 ml Flow rate: 7.62 L/min: Pulse count: 61 Pulse Frequency: 29.41 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 28043 WaterFlow: 0.00 ml Flow rate: 8.33 L/min: Pulse count: 78 Pulse Frequency: 32.26 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 28584 WaterFlow: 0.00 ml Flow rate: 9.20 L/min: Pulse count: 96 Pulse Frequency: 32.26 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 29126 WaterFlow: 0.00 ml Flow rate: 8.89 L/min: Pulse count: 114 Pulse Frequency: 34.48 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 29669 WaterFlow: 0.00 ml Flow rate: 8.89 L/min: Pulse count: 133 Pulse Frequency: 34.48 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 30212 WaterFlow: 0.00 ml Flow rate: 8.89 L/min: Pulse count: 151 Pulse Frequency: 34.48 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 30754 WaterFlow: 0.00 ml Flow rate: 8.89 L/min: Pulse count: 170 Pulse Frequency: 33.33 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 31297 WaterFlow: 0.00 ml Flow rate: 9.20 L/min: Pulse count: 188 Pulse Frequency: 34.48 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 31840 WaterFlow: 0.00 ml Flow rate: 9.52 L/min: Pulse count: 206 Pulse Frequency: 32.26 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 32382 WaterFlow: 0.00 ml Flow rate: 8.89 L/min: Pulse count: 225 Pulse Frequency: 33.33 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 32925 WaterFlow: 0.00 ml Flow rate: 9.20 L/min: Pulse count: 243 Pulse Frequency: 33.33 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 33468 WaterFlow: 0.00 ml Flow rate: 9.20 L/min: Pulse count: 261 Pulse Frequency: 32.26 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 34011 WaterFlow: 0.00 ml Flow rate: 9.20 L/min: Pulse count: 278 Pulse Frequency: 32.26 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 34553 WaterFlow: 0.00 ml Flow rate: 8.89 L/min: Pulse count: 296 Pulse Frequency: 32.26 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 35096 WaterFlow: 0.00 ml Flow rate: 8.89 L/min: Pulse count: 314 Pulse Frequency: 32.26 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 35639 WaterFlow: 0.00 ml Flow rate: 8.60 L/min: Pulse count: 332 Pulse Frequency: 33.33 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 36182 WaterFlow: 0.00 ml Flow rate: 8.33 L/min: Pulse count: 350 Pulse Frequency: 33.33 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 36724 WaterFlow: 0.00 ml Flow rate: 8.60 L/min: Pulse count: 367 Pulse Frequency: 32.26 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 37267 WaterFlow: 0.00 ml Flow rate: 8.89 L/min: Pulse count: 385 Pulse Frequency: 31.25 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 37810 WaterFlow: 0.00 ml Flow rate: 8.33 L/min: Pulse count: 402 Pulse Frequency: 32.26 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 38352 WaterFlow: 0.00 ml Flow rate: 8.60 L/min: Pulse count: 419 Pulse Frequency: 31.25 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 38895 WaterFlow: 0.00 ml Flow rate: 8.33 L/min: Pulse count: 437 Pulse Frequency: 33.33 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 39438 WaterFlow: 0.00 ml Flow rate: 8.33 L/min: Pulse count: 454 Pulse Frequency: 32.26 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 39981 WaterFlow: 0.00 ml Flow rate: 8.60 L/min: Pulse count: 471 Pulse Frequency: 30.30 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 40523 WaterFlow: 0.00 ml Flow rate: 8.33 L/min: Pulse count: 488 Pulse Frequency: 30.30 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 41066 WaterFlow: 0.00 ml Flow rate: 8.33 L/min: Pulse count: 505 Pulse Frequency: 30.30 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 41609 WaterFlow: 0.00 ml Flow rate: 8.33 L/min: Pulse count: 521 Pulse Frequency: 30.30 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 42151 WaterFlow: 0.00 ml Flow rate: 8.33 L/min: Pulse count: 538 Pulse Frequency: 30.30 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 42694 WaterFlow: 0.00 ml Flow rate: 8.08 L/min: Pulse count: 555 Pulse Frequency: 30.30 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 43237 WaterFlow: 0.00 ml Flow rate: 8.33 L/min: Pulse count: 571 Pulse Frequency: 30.30 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 43780 WaterFlow: 0.00 ml Flow rate: 7.84 L/min: Pulse count: 588 Pulse Frequency: 31.25 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 44322 WaterFlow: 0.00 ml Flow rate: 8.08 L/min: Pulse count: 604 Pulse Frequency: 30.30 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 44865 WaterFlow: 0.00 ml Flow rate: 8.33 L/min: Pulse count: 621 Pulse Frequency: 29.41 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 45408 WaterFlow: 0.00 ml Flow rate: 7.84 L/min: Pulse count: 637 Pulse Frequency: 30.30 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 45950 WaterFlow: 0.00 ml Flow rate: 8.33 L/min: Pulse count: 653 Pulse Frequency: 28.57 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 46493 WaterFlow: 0.00 ml Flow rate: 7.62 L/min: Pulse count: 669 Pulse Frequency: 29.41 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 47036 WaterFlow: 0.00 ml Flow rate: 7.62 L/min: Pulse count: 685 Pulse Frequency: 29.41 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 47579 WaterFlow: 0.00 ml Flow rate: 7.21 L/min: Pulse count: 700 Pulse Frequency: 27.78 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 48121 WaterFlow: 0.00 ml Flow rate: 7.41 L/min: Pulse count: 715 Pulse Frequency: 27.78 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 48664 WaterFlow: 0.00 ml Flow rate: 7.21 L/min: Pulse count: 730 Pulse Frequency: 27.78 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 49207 WaterFlow: 0.00 ml Flow rate: 7.02 L/min: Pulse count: 745 Pulse Frequency: 26.32 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 49750 WaterFlow: 0.00 ml Flow rate: 6.20 L/min: Pulse count: 758 Pulse Frequency: 22.73 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 50292 WaterFlow: 0.00 ml Flow rate: 4.04 L/min: Pulse count: 769 Pulse Frequency: 15.15 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Time: 50835 WaterFlow: 0.00 ml Flow rate: 2.52 L/min: Pulse count: 770 Pulse Frequency: 9.43 Hz: </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 23177 Pulse count: 1 Pulse Frequency: 0.04 Hz: </t>
+  </si>
+  <si>
+    <t>Time</t>
   </si>
 </sst>
 </file>
@@ -98,6 +274,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -136,7 +317,7 @@
           </c:trendline>
           <c:trendline>
             <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
+            <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout/>
@@ -231,11 +412,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2110860984"/>
-        <c:axId val="-2109126984"/>
+        <c:axId val="1428862480"/>
+        <c:axId val="1428864800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2110860984"/>
+        <c:axId val="1428862480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -245,12 +426,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2109126984"/>
+        <c:crossAx val="1428864800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2109126984"/>
+        <c:axId val="1428864800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -261,7 +442,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2110860984"/>
+        <c:crossAx val="1428862480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -283,20 +464,1102 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="47625" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.118791338582677"/>
+                  <c:y val="-0.0050462962962963"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$N$29:$N$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1450.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>653.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>253.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>369.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>966.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1774.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>702.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>577.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>594.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>785.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>673.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1215.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>839.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>790.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>510.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$O$29:$O$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>375.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>180.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>258.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>450.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>195.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>180.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>180.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>225.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>190.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>320.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>240.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>225.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1479147408"/>
+        <c:axId val="1479144400"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1479147408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Pulse Counts</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1479144400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1479144400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Water Volume (ml)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1479147408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -310,6 +1573,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -640,20 +1933,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:S61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" activeCellId="1" sqref="A2:A11 C2:C11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.83203125" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="19" max="19" width="95" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -663,8 +1957,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>50</v>
       </c>
@@ -679,7 +1976,7 @@
         <v>1.4556040756914119</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3">
         <f>A2+50</f>
         <v>100</v>
@@ -695,7 +1992,7 @@
         <v>1.5849116411760045</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" ref="A4:A11" si="0">A3+50</f>
         <v>150</v>
@@ -711,7 +2008,7 @@
         <v>1.413494157557482</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>200</v>
@@ -723,7 +2020,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -735,7 +2032,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>300</v>
@@ -747,7 +2044,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>350</v>
@@ -759,7 +2056,7 @@
         <v>1436</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>400</v>
@@ -770,8 +2067,14 @@
       <c r="C9">
         <v>1771</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="Q9" t="s">
+        <v>59</v>
+      </c>
+      <c r="R9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>450</v>
@@ -782,8 +2085,11 @@
       <c r="C10">
         <v>2010</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="S10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>500</v>
@@ -794,20 +2100,741 @@
       <c r="C11">
         <v>2233</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="S11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>3</v>
+      </c>
+      <c r="S12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>0</v>
+      </c>
+      <c r="H21" t="s">
+        <v>6</v>
+      </c>
+      <c r="S21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>375</v>
+      </c>
+      <c r="B22">
+        <v>246.6</v>
+      </c>
+      <c r="C22">
+        <v>1450</v>
+      </c>
+      <c r="D22">
+        <v>375</v>
+      </c>
+      <c r="G22">
+        <f>C22/B22</f>
+        <v>5.8799675587996756</v>
+      </c>
+      <c r="H22">
+        <f>C22/A22</f>
+        <v>3.8666666666666667</v>
+      </c>
+      <c r="S22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>180</v>
+      </c>
+      <c r="B23">
+        <f>357.66-246.6</f>
+        <v>111.06000000000003</v>
+      </c>
+      <c r="C23">
+        <f>2103-1450</f>
+        <v>653</v>
+      </c>
+      <c r="D23">
+        <v>180</v>
+      </c>
+      <c r="G23">
+        <f t="shared" ref="G23:G33" si="1">C23/B23</f>
+        <v>5.8797046641455051</v>
+      </c>
+      <c r="H23">
+        <f t="shared" ref="H23:H33" si="2">C23/A23</f>
+        <v>3.6277777777777778</v>
+      </c>
+      <c r="S23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>80</v>
+      </c>
+      <c r="B24">
+        <v>43.03</v>
+      </c>
+      <c r="C24">
+        <v>253</v>
+      </c>
+      <c r="D24">
+        <v>80</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>5.8796188705554266</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="2"/>
+        <v>3.1625000000000001</v>
+      </c>
+      <c r="S24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>100</v>
+      </c>
+      <c r="B25">
+        <v>62.75</v>
+      </c>
+      <c r="C25">
+        <v>369</v>
+      </c>
+      <c r="D25">
+        <v>100</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>5.8804780876494025</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="2"/>
+        <v>3.69</v>
+      </c>
+      <c r="S25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>258</v>
+      </c>
+      <c r="B26">
+        <v>164.29</v>
+      </c>
+      <c r="C26">
+        <v>966</v>
+      </c>
+      <c r="D26">
+        <v>258</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>5.8798466126970608</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="2"/>
+        <v>3.7441860465116279</v>
+      </c>
+      <c r="S26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>500</v>
+      </c>
+      <c r="B27">
+        <v>562.41999999999996</v>
+      </c>
+      <c r="C27">
+        <v>3307</v>
+      </c>
+      <c r="D27">
+        <v>500</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>5.8799473702926646</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="2"/>
+        <v>6.6139999999999999</v>
+      </c>
+      <c r="S27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>450</v>
+      </c>
+      <c r="B28">
+        <v>301.70999999999998</v>
+      </c>
+      <c r="C28">
+        <v>1774</v>
+      </c>
+      <c r="D28">
+        <v>450</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>5.8798183686321304</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="2"/>
+        <v>3.9422222222222221</v>
+      </c>
+      <c r="S28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>195</v>
+      </c>
+      <c r="B29">
+        <f>421.1-301.71</f>
+        <v>119.39000000000004</v>
+      </c>
+      <c r="C29">
+        <f>2476-1774</f>
+        <v>702</v>
+      </c>
+      <c r="D29">
+        <v>195</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>5.8798894379763782</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="2"/>
+        <v>3.6</v>
+      </c>
+      <c r="N29">
+        <v>1450</v>
+      </c>
+      <c r="O29">
+        <v>375</v>
+      </c>
+      <c r="S29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>180</v>
+      </c>
+      <c r="B30">
+        <v>98.13</v>
+      </c>
+      <c r="C30">
+        <v>577</v>
+      </c>
+      <c r="D30">
+        <v>180</v>
+      </c>
+      <c r="E30" t="s">
+        <v>5</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="1"/>
+        <v>5.8799551615204324</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="2"/>
+        <v>3.2055555555555557</v>
+      </c>
+      <c r="N30">
+        <f>2103-1450</f>
+        <v>653</v>
+      </c>
+      <c r="O30">
+        <v>180</v>
+      </c>
+      <c r="S30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>180</v>
+      </c>
+      <c r="B31">
+        <f>199.15-98.13</f>
+        <v>101.02000000000001</v>
+      </c>
+      <c r="C31">
+        <f>1171-577</f>
+        <v>594</v>
+      </c>
+      <c r="D31">
+        <v>180</v>
+      </c>
+      <c r="E31" t="s">
+        <v>5</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="1"/>
+        <v>5.880023757671748</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="2"/>
+        <v>3.3</v>
+      </c>
+      <c r="N31">
+        <v>253</v>
+      </c>
+      <c r="O31">
+        <v>80</v>
+      </c>
+      <c r="S31" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>225</v>
+      </c>
+      <c r="B32">
+        <v>133.5</v>
+      </c>
+      <c r="C32">
+        <v>785</v>
+      </c>
+      <c r="D32">
+        <v>225</v>
+      </c>
+      <c r="E32" t="s">
+        <v>5</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="1"/>
+        <v>5.8801498127340821</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="2"/>
+        <v>3.4888888888888889</v>
+      </c>
+      <c r="N32">
+        <v>369</v>
+      </c>
+      <c r="O32">
+        <v>100</v>
+      </c>
+      <c r="S32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>190</v>
+      </c>
+      <c r="B33">
+        <v>114</v>
+      </c>
+      <c r="C33">
+        <v>673</v>
+      </c>
+      <c r="D33">
+        <v>190</v>
+      </c>
+      <c r="G33">
+        <f>C33/B33</f>
+        <v>5.9035087719298245</v>
+      </c>
+      <c r="H33">
+        <f>C33/A33</f>
+        <v>3.5421052631578949</v>
+      </c>
+      <c r="N33">
+        <v>966</v>
+      </c>
+      <c r="O33">
+        <v>258</v>
+      </c>
+      <c r="S33" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>320</v>
+      </c>
+      <c r="B34">
+        <v>341.2</v>
+      </c>
+      <c r="C34">
+        <v>1215</v>
+      </c>
+      <c r="D34">
+        <v>320</v>
+      </c>
+      <c r="G34">
+        <f>C34/B34</f>
+        <v>3.5609613130128959</v>
+      </c>
+      <c r="H34">
+        <f t="shared" ref="H34:H39" si="3">C34/A34</f>
+        <v>3.796875</v>
+      </c>
+      <c r="N34">
+        <v>1774</v>
+      </c>
+      <c r="O34">
+        <v>450</v>
+      </c>
+      <c r="S34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>240</v>
+      </c>
+      <c r="B35">
+        <v>238.42</v>
+      </c>
+      <c r="C35">
+        <v>839</v>
+      </c>
+      <c r="D35">
+        <v>240</v>
+      </c>
+      <c r="G35">
+        <f t="shared" ref="G35:G38" si="4">C35/B35</f>
+        <v>3.5190000838855804</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="3"/>
+        <v>3.4958333333333331</v>
+      </c>
+      <c r="N35">
+        <f>2476-1774</f>
+        <v>702</v>
+      </c>
+      <c r="O35">
+        <v>195</v>
+      </c>
+      <c r="S35" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>225</v>
+      </c>
+      <c r="B36">
+        <v>221.85</v>
+      </c>
+      <c r="C36">
+        <v>790</v>
+      </c>
+      <c r="D36">
+        <v>225</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="4"/>
+        <v>3.5609646157313501</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="3"/>
+        <v>3.5111111111111111</v>
+      </c>
+      <c r="N36">
+        <v>577</v>
+      </c>
+      <c r="O36">
+        <v>180</v>
+      </c>
+      <c r="S36" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>150</v>
+      </c>
+      <c r="B37">
+        <v>143.22</v>
+      </c>
+      <c r="C37">
+        <v>510</v>
+      </c>
+      <c r="D37">
+        <v>150</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="4"/>
+        <v>3.5609551738583995</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="3"/>
+        <v>3.4</v>
+      </c>
+      <c r="N37">
+        <f>1171-577</f>
+        <v>594</v>
+      </c>
+      <c r="O37">
+        <v>180</v>
+      </c>
+      <c r="S37" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>500</v>
+      </c>
+      <c r="B38">
+        <v>532</v>
+      </c>
+      <c r="C38">
+        <v>2090</v>
+      </c>
+      <c r="D38">
+        <v>500</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="4"/>
+        <v>3.9285714285714284</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="3"/>
+        <v>4.18</v>
+      </c>
+      <c r="N38">
+        <v>785</v>
+      </c>
+      <c r="O38">
+        <v>225</v>
+      </c>
+      <c r="S38" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="H39" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N39">
+        <v>673</v>
+      </c>
+      <c r="O39">
+        <v>190</v>
+      </c>
+      <c r="S39" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="N40">
+        <v>1215</v>
+      </c>
+      <c r="O40">
+        <v>320</v>
+      </c>
+      <c r="S40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="N41">
+        <v>839</v>
+      </c>
+      <c r="O41">
+        <v>240</v>
+      </c>
+      <c r="S41" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="H42">
+        <f>AVERAGE(H22:H33)</f>
+        <v>3.815325201731719</v>
+      </c>
+      <c r="I42">
+        <f>AVERAGE(H22:H26,H28:H36)</f>
+        <v>3.569551561801791</v>
+      </c>
+      <c r="N42">
+        <v>790</v>
+      </c>
+      <c r="O42">
+        <v>225</v>
+      </c>
+      <c r="S42" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="N43">
+        <v>510</v>
+      </c>
+      <c r="O43">
+        <v>150</v>
+      </c>
+      <c r="S43" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S44" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S45" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S46" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S47" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S48" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="49" spans="19:19" x14ac:dyDescent="0.2">
+      <c r="S49" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="19:19" x14ac:dyDescent="0.2">
+      <c r="S50" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="51" spans="19:19" x14ac:dyDescent="0.2">
+      <c r="S51" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="52" spans="19:19" x14ac:dyDescent="0.2">
+      <c r="S52" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="53" spans="19:19" x14ac:dyDescent="0.2">
+      <c r="S53" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="54" spans="19:19" x14ac:dyDescent="0.2">
+      <c r="S54" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="19:19" x14ac:dyDescent="0.2">
+      <c r="S55" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="56" spans="19:19" x14ac:dyDescent="0.2">
+      <c r="S56" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="57" spans="19:19" x14ac:dyDescent="0.2">
+      <c r="S57" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="58" spans="19:19" x14ac:dyDescent="0.2">
+      <c r="S58" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="59" spans="19:19" x14ac:dyDescent="0.2">
+      <c r="S59" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="60" spans="19:19" x14ac:dyDescent="0.2">
+      <c r="S60" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="61" spans="19:19" x14ac:dyDescent="0.2">
+      <c r="S61" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>